<commit_message>
DA 21 | Practise Questions
</commit_message>
<xml_diff>
--- a/batches/21/week_01_foundations_environment/day_03/day_3.xlsx
+++ b/batches/21/week_01_foundations_environment/day_03/day_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shira/Documents/modules/sql/batches/21/week_01_foundations_environment/day_03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59470798-1883-8E40-93A6-7E7C61EC30D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78E5B70-C5A9-C34C-9985-8965A8001C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1440" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{E6A878E2-DFBC-9542-9166-5715E9949272}"/>
+    <workbookView xWindow="-38400" yWindow="-940" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{E6A878E2-DFBC-9542-9166-5715E9949272}"/>
   </bookViews>
   <sheets>
     <sheet name="Recap" sheetId="1" r:id="rId1"/>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00B976C6-FFA2-D247-89E0-640817255AC2}">
   <dimension ref="B2:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="268" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:C33"/>
+    <sheetView topLeftCell="A12" zoomScale="268" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -857,7 +857,7 @@
   <dimension ref="A2:C13"/>
   <sheetViews>
     <sheetView zoomScale="303" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1064,7 +1064,7 @@
   <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="276" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>